<commit_message>
pruebas y mejoras ordenes en tandem
</commit_message>
<xml_diff>
--- a/DOCS/Pendientes Trader Prod.xlsx
+++ b/DOCS/Pendientes Trader Prod.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="120" windowWidth="17715" windowHeight="4170"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
   <si>
     <t>Pendientes Kraken Trader PROD</t>
   </si>
@@ -356,13 +356,16 @@
   </si>
   <si>
     <t>listo</t>
+  </si>
+  <si>
+    <t>desarrolando</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,6 +398,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -528,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -575,6 +584,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,7 +675,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -699,7 +709,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -875,21 +884,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H5" sqref="H1:H1048576"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="94.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -901,8 +910,8 @@
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -928,7 +937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="22" t="s">
         <v>63</v>
       </c>
@@ -940,7 +949,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -954,7 +963,7 @@
       <c r="E5" s="18">
         <v>43061</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="26" t="s">
         <v>85</v>
       </c>
       <c r="G5" s="18">
@@ -962,7 +971,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -976,7 +985,7 @@
       <c r="E6" s="18">
         <v>43061</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="26" t="s">
         <v>85</v>
       </c>
       <c r="G6" s="18">
@@ -986,7 +995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="20" t="s">
         <v>80</v>
       </c>
@@ -1002,7 +1011,7 @@
       <c r="E7" s="18">
         <v>43065</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="26" t="s">
         <v>85</v>
       </c>
       <c r="G7" s="18">
@@ -1010,7 +1019,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -1026,7 +1035,7 @@
       <c r="E8" s="18">
         <v>43061</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="26" t="s">
         <v>85</v>
       </c>
       <c r="G8" s="18">
@@ -1036,7 +1045,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="21" t="s">
         <v>82</v>
       </c>
@@ -1052,7 +1061,7 @@
       <c r="E9" s="18">
         <v>43073</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="26" t="s">
         <v>85</v>
       </c>
       <c r="G9" s="18">
@@ -1062,7 +1071,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="21" t="s">
         <v>86</v>
       </c>
@@ -1084,7 +1093,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="21" t="s">
         <v>89</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="3">
         <v>4</v>
       </c>
@@ -1120,7 +1129,7 @@
       <c r="E12" s="18">
         <v>43061</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="26" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="18">
@@ -1130,7 +1139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="21" t="s">
         <v>102</v>
       </c>
@@ -1150,7 +1159,7 @@
       <c r="G13" s="18"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="21" t="s">
         <v>104</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="21">
         <v>5</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="3">
         <v>6</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="3">
         <v>7</v>
       </c>
@@ -1244,7 +1253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="3">
         <v>8</v>
       </c>
@@ -1268,7 +1277,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="21" t="s">
         <v>107</v>
       </c>
@@ -1280,15 +1289,15 @@
       <c r="E19" s="18">
         <v>43078</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>12</v>
+      <c r="F19" s="27" t="s">
+        <v>113</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="21" t="s">
         <v>92</v>
       </c>
@@ -1312,7 +1321,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="21" t="s">
         <v>95</v>
       </c>
@@ -1334,7 +1343,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="21" t="s">
         <v>98</v>
       </c>
@@ -1358,7 +1367,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="3">
         <v>9</v>
       </c>
@@ -1382,7 +1391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="3">
         <v>10</v>
       </c>
@@ -1406,7 +1415,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="3">
         <v>11</v>
       </c>
@@ -1430,7 +1439,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="3">
         <v>12</v>
       </c>
@@ -1454,7 +1463,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="3">
         <v>13</v>
       </c>
@@ -1478,7 +1487,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="3">
         <v>14</v>
       </c>
@@ -1492,7 +1501,7 @@
       <c r="E28" s="18">
         <v>43061</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="26" t="s">
         <v>112</v>
       </c>
       <c r="G28" s="18">
@@ -1502,7 +1511,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="3">
         <v>15</v>
       </c>
@@ -1518,7 +1527,7 @@
       <c r="E29" s="18">
         <v>43061</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="26" t="s">
         <v>112</v>
       </c>
       <c r="G29" s="18">
@@ -1528,7 +1537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="3">
         <v>16</v>
       </c>
@@ -1544,7 +1553,7 @@
       <c r="E30" s="18">
         <v>43061</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="26" t="s">
         <v>112</v>
       </c>
       <c r="G30" s="18">
@@ -1554,7 +1563,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="3">
         <v>17</v>
       </c>
@@ -1576,7 +1585,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="3">
         <v>18</v>
       </c>
@@ -1598,7 +1607,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="3">
         <v>19</v>
       </c>
@@ -1620,7 +1629,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="3">
         <v>21</v>
       </c>
@@ -1644,7 +1653,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="15.75" thickBot="1">
       <c r="A35" s="6">
         <v>22</v>
       </c>
@@ -1668,8 +1677,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1">
       <c r="A37" s="22" t="s">
         <v>62</v>
       </c>
@@ -1681,7 +1690,7 @@
       <c r="G37" s="23"/>
       <c r="H37" s="24"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="3">
         <v>23</v>
       </c>
@@ -1703,7 +1712,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="3">
         <v>24</v>
       </c>
@@ -1725,7 +1734,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="3">
         <v>25</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="3">
         <v>26</v>
       </c>
@@ -1771,7 +1780,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="3">
         <v>27</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="15.75" thickBot="1">
       <c r="A43" s="6">
         <v>28</v>
       </c>
@@ -1819,8 +1828,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1">
       <c r="A45" s="22" t="s">
         <v>65</v>
       </c>
@@ -1832,7 +1841,7 @@
       <c r="G45" s="23"/>
       <c r="H45" s="24"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="3">
         <v>29</v>
       </c>
@@ -1854,7 +1863,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="3">
         <v>30</v>
       </c>
@@ -1876,7 +1885,7 @@
       <c r="G47" s="4"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="3">
         <v>31</v>
       </c>
@@ -1898,7 +1907,7 @@
       <c r="G48" s="4"/>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="3">
         <v>32</v>
       </c>
@@ -1920,7 +1929,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="45.75" thickBot="1">
       <c r="A50" s="13">
         <v>33</v>
       </c>
@@ -1944,8 +1953,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1">
       <c r="A52" s="22" t="s">
         <v>73</v>
       </c>
@@ -1957,7 +1966,7 @@
       <c r="G52" s="23"/>
       <c r="H52" s="24"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="10">
         <v>34</v>
       </c>
@@ -1975,7 +1984,7 @@
       <c r="G53" s="11"/>
       <c r="H53" s="12"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="3">
         <v>35</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="15.75" thickBot="1">
       <c r="A55" s="6">
         <v>36</v>
       </c>
@@ -2013,7 +2022,7 @@
       <c r="G55" s="7"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="17">
         <v>37</v>
       </c>
@@ -2040,24 +2049,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
incorporado order manaer aun no funcional evaluacion online funcional save profit y reopen funcional
</commit_message>
<xml_diff>
--- a/DOCS/Pendientes Trader Prod.xlsx
+++ b/DOCS/Pendientes Trader Prod.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="120" windowWidth="17715" windowHeight="4170"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="124">
   <si>
     <t>Pendientes Kraken Trader PROD</t>
   </si>
@@ -358,14 +358,44 @@
     <t>listo</t>
   </si>
   <si>
-    <t>desarrolando</t>
+    <t>otras mejoras recomendables</t>
+  </si>
+  <si>
+    <t>mejorar tolerancia maximo tolerado, al salbar ganancias y reabrir operación en tanden, la oeracion se sale prematuramente por maximo tolerado muy ajustado.</t>
+  </si>
+  <si>
+    <t>separar myTreades y MyTradesBackTest, por un comportamieto desconosido de SQLalchemy, no toma el nombre de la tabla MyTradesBackTest, al guargar y actualesar las operacioens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorporat tolerancia ante caidas momentanes , por la variacion promedio del mercado, ya sea or conteo de tiempo que el % de CH es peligroso, o por conteo de periodos , por ejemplo cuenta regresiva. </t>
+  </si>
+  <si>
+    <t>agregar mas CRYPTOs y otros agentes para ampliar el marcado</t>
+  </si>
+  <si>
+    <t>manejar slot de ordenes y operaciones en simultaneso</t>
+  </si>
+  <si>
+    <t>ver como si combiene comvetuirse en un miner de cryptos</t>
+  </si>
+  <si>
+    <t>comprar un servidor</t>
+  </si>
+  <si>
+    <t>comprar una ups</t>
+  </si>
+  <si>
+    <t>comprar un monitor</t>
+  </si>
+  <si>
+    <t>ver que es mas rentable/combeniente, subir a servidor en google cloud o ejecuta ren servido rpropio dedicado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,12 +428,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,6 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -584,8 +609,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,6 +699,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -709,6 +734,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -884,34 +910,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="94.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -937,19 +963,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -963,7 +989,7 @@
       <c r="E5" s="18">
         <v>43061</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G5" s="18">
@@ -971,7 +997,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -985,7 +1011,7 @@
       <c r="E6" s="18">
         <v>43061</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G6" s="18">
@@ -995,7 +1021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>80</v>
       </c>
@@ -1011,7 +1037,7 @@
       <c r="E7" s="18">
         <v>43065</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G7" s="18">
@@ -1019,7 +1045,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>3</v>
       </c>
@@ -1035,7 +1061,7 @@
       <c r="E8" s="18">
         <v>43061</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G8" s="18">
@@ -1045,7 +1071,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>82</v>
       </c>
@@ -1061,7 +1087,7 @@
       <c r="E9" s="18">
         <v>43073</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G9" s="18">
@@ -1071,7 +1097,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>86</v>
       </c>
@@ -1093,7 +1119,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>89</v>
       </c>
@@ -1115,7 +1141,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>4</v>
       </c>
@@ -1129,7 +1155,7 @@
       <c r="E12" s="18">
         <v>43061</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="18">
@@ -1139,7 +1165,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>102</v>
       </c>
@@ -1159,7 +1185,7 @@
       <c r="G13" s="18"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>104</v>
       </c>
@@ -1181,7 +1207,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>5</v>
       </c>
@@ -1205,7 +1231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>6</v>
       </c>
@@ -1229,7 +1255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>7</v>
       </c>
@@ -1253,7 +1279,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>8</v>
       </c>
@@ -1277,7 +1303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>107</v>
       </c>
@@ -1289,15 +1315,17 @@
       <c r="E19" s="18">
         <v>43078</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="4"/>
+      <c r="F19" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="18">
+        <v>43091</v>
+      </c>
       <c r="H19" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>92</v>
       </c>
@@ -1321,7 +1349,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>95</v>
       </c>
@@ -1343,7 +1371,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>98</v>
       </c>
@@ -1367,7 +1395,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>9</v>
       </c>
@@ -1391,7 +1419,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>10</v>
       </c>
@@ -1415,7 +1443,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>11</v>
       </c>
@@ -1439,7 +1467,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>12</v>
       </c>
@@ -1463,7 +1491,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>13</v>
       </c>
@@ -1487,7 +1515,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>14</v>
       </c>
@@ -1501,7 +1529,7 @@
       <c r="E28" s="18">
         <v>43061</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="22" t="s">
         <v>112</v>
       </c>
       <c r="G28" s="18">
@@ -1511,7 +1539,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>15</v>
       </c>
@@ -1527,7 +1555,7 @@
       <c r="E29" s="18">
         <v>43061</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="22" t="s">
         <v>112</v>
       </c>
       <c r="G29" s="18">
@@ -1537,7 +1565,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>16</v>
       </c>
@@ -1553,7 +1581,7 @@
       <c r="E30" s="18">
         <v>43061</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="22" t="s">
         <v>112</v>
       </c>
       <c r="G30" s="18">
@@ -1563,7 +1591,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>17</v>
       </c>
@@ -1585,7 +1613,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>18</v>
       </c>
@@ -1607,7 +1635,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>19</v>
       </c>
@@ -1629,7 +1657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>21</v>
       </c>
@@ -1653,7 +1681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1">
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>22</v>
       </c>
@@ -1677,20 +1705,20 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1"/>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A37" s="22" t="s">
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="24"/>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="25"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>23</v>
       </c>
@@ -1712,7 +1740,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>24</v>
       </c>
@@ -1734,7 +1762,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>25</v>
       </c>
@@ -1756,7 +1784,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>26</v>
       </c>
@@ -1780,7 +1808,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>27</v>
       </c>
@@ -1804,7 +1832,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1">
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>28</v>
       </c>
@@ -1828,20 +1856,20 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1"/>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A45" s="22" t="s">
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="24"/>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="25"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>29</v>
       </c>
@@ -1863,7 +1891,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>30</v>
       </c>
@@ -1885,7 +1913,7 @@
       <c r="G47" s="4"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>31</v>
       </c>
@@ -1907,7 +1935,7 @@
       <c r="G48" s="4"/>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>32</v>
       </c>
@@ -1929,7 +1957,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45.75" thickBot="1">
+    <row r="50" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>33</v>
       </c>
@@ -1953,20 +1981,20 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" thickBot="1"/>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A52" s="22" t="s">
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="24"/>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="25"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>34</v>
       </c>
@@ -1984,7 +2012,7 @@
       <c r="G53" s="11"/>
       <c r="H53" s="12"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>35</v>
       </c>
@@ -2004,7 +2032,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1">
+    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>36</v>
       </c>
@@ -2022,7 +2050,7 @@
       <c r="G55" s="7"/>
       <c r="H55" s="8"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>37</v>
       </c>
@@ -2035,8 +2063,72 @@
       <c r="F57" s="17"/>
       <c r="G57" s="17"/>
     </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="25"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A60:H60"/>
     <mergeCell ref="A52:H52"/>
     <mergeCell ref="A45:H45"/>
     <mergeCell ref="A37:H37"/>
@@ -2049,24 +2141,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bug en trade close y reopen
</commit_message>
<xml_diff>
--- a/DOCS/Pendientes Trader Prod.xlsx
+++ b/DOCS/Pendientes Trader Prod.xlsx
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
aumentado time out bbdd. Incorporado eliminacio de TradesHistory para mejora de performance
</commit_message>
<xml_diff>
--- a/DOCS/Pendientes Trader Prod.xlsx
+++ b/DOCS/Pendientes Trader Prod.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="129">
   <si>
     <t>Pendientes Kraken Trader PROD</t>
   </si>
@@ -289,9 +289,6 @@
     <t>3.4</t>
   </si>
   <si>
-    <t>crear scrip Trader.Main multitread</t>
-  </si>
-  <si>
     <t>registrar maximo op y reajustar maximoTolerado según rendimiento</t>
   </si>
   <si>
@@ -395,13 +392,25 @@
   </si>
   <si>
     <t>desarrollo</t>
+  </si>
+  <si>
+    <t>crear script Trader.Main multitread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abrir operación y crear orden de compra manual </t>
+  </si>
+  <si>
+    <t>cerrar operación y crear orden de venta manual</t>
+  </si>
+  <si>
+    <t>corregir profit y profit -gastos , agregar soporte caida y reinico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +422,14 @@
       <b/>
       <sz val="14"/>
       <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -579,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -615,6 +632,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -627,14 +652,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,16 +968,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -989,16 +1007,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -1101,7 +1119,7 @@
         <v>82</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="19">
         <v>2</v>
@@ -1149,7 +1167,7 @@
         <v>89</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="19">
         <v>3</v>
@@ -1163,7 +1181,7 @@
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1192,10 +1210,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="C13" s="19">
         <v>1</v>
@@ -1212,10 +1230,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>104</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>105</v>
       </c>
       <c r="C14" s="19">
         <v>2</v>
@@ -1224,12 +1242,12 @@
       <c r="E14" s="18">
         <v>43078</v>
       </c>
-      <c r="F14" s="30" t="s">
-        <v>125</v>
+      <c r="F14" s="26" t="s">
+        <v>124</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1248,8 +1266,8 @@
       <c r="E15" s="18">
         <v>43061</v>
       </c>
-      <c r="F15" s="30" t="s">
-        <v>125</v>
+      <c r="F15" s="26" t="s">
+        <v>124</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="5" t="s">
@@ -1272,10 +1290,12 @@
       <c r="E16" s="18">
         <v>43061</v>
       </c>
-      <c r="F16" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="G16" s="4"/>
+      <c r="F16" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="18">
+        <v>43095</v>
+      </c>
       <c r="H16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1330,10 +1350,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1347,15 +1367,15 @@
         <v>43091</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>93</v>
       </c>
       <c r="C20" s="19">
         <v>2</v>
@@ -1371,15 +1391,15 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="19">
         <v>3</v>
@@ -1388,26 +1408,26 @@
       <c r="E21" s="18">
         <v>43074</v>
       </c>
-      <c r="F21" s="30" t="s">
-        <v>125</v>
+      <c r="F21" s="26" t="s">
+        <v>124</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="19">
         <v>2</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E22" s="18">
         <v>43074</v>
@@ -1417,7 +1437,7 @@
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,10 +1456,12 @@
       <c r="E23" s="18">
         <v>43061</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="4"/>
+      <c r="F23" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="18">
+        <v>43095</v>
+      </c>
       <c r="H23" s="5" t="s">
         <v>19</v>
       </c>
@@ -1545,7 +1567,7 @@
         <v>14</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="C28" s="4">
         <v>1</v>
@@ -1555,7 +1577,7 @@
         <v>43061</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G28" s="18">
         <v>43089</v>
@@ -1581,7 +1603,7 @@
         <v>43061</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G29" s="18">
         <v>43089</v>
@@ -1607,7 +1629,7 @@
         <v>43061</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G30" s="18">
         <v>43089</v>
@@ -1617,55 +1639,43 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>17</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="4">
-        <v>2</v>
+      <c r="A31" s="3"/>
+      <c r="B31" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="19">
+        <v>3</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="5" t="s">
-        <v>44</v>
-      </c>
+        <v>43099</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>18</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2</v>
+      <c r="A32" s="3"/>
+      <c r="B32" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="19">
+        <v>3</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="5" t="s">
-        <v>44</v>
-      </c>
+        <v>43099</v>
+      </c>
+      <c r="F32" s="19"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C33" s="4">
         <v>2</v>
@@ -1679,22 +1689,20 @@
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C34" s="4">
         <v>2</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="D34" s="4"/>
       <c r="E34" s="18">
         <v>43061</v>
       </c>
@@ -1703,96 +1711,98 @@
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>19</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>21</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
         <v>22</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C37" s="7">
         <v>2</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="8" t="s">
+      <c r="E37" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="25"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>23</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="4">
-        <v>4</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>24</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="4">
-        <v>4</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="5" t="s">
-        <v>56</v>
-      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="29"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C40" s="4">
         <v>4</v>
@@ -1806,22 +1816,20 @@
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C41" s="4">
         <v>4</v>
       </c>
-      <c r="D41" s="4">
-        <v>25</v>
-      </c>
+      <c r="D41" s="4"/>
       <c r="E41" s="18">
         <v>43061</v>
       </c>
@@ -1830,22 +1838,20 @@
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C42" s="4">
         <v>4</v>
       </c>
-      <c r="D42" s="4">
-        <v>25</v>
-      </c>
+      <c r="D42" s="4"/>
       <c r="E42" s="18">
         <v>43061</v>
       </c>
@@ -1854,103 +1860,105 @@
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>26</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="4">
+        <v>4</v>
+      </c>
+      <c r="D43" s="4">
+        <v>25</v>
+      </c>
+      <c r="E43" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="4"/>
+      <c r="H43" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>27</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="4">
+        <v>4</v>
+      </c>
+      <c r="D44" s="4">
+        <v>25</v>
+      </c>
+      <c r="E44" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="6">
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
         <v>28</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C45" s="7">
         <v>4</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D45" s="7">
         <v>25</v>
       </c>
-      <c r="E43" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G43" s="7"/>
-      <c r="H43" s="8" t="s">
+      <c r="E45" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="7"/>
+      <c r="H45" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="23" t="s">
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="25"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>29</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="4">
-        <v>3</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>30</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="4">
-        <v>3</v>
-      </c>
-      <c r="D47" s="4">
-        <v>29</v>
-      </c>
-      <c r="E47" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="4"/>
-      <c r="H47" s="5"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="29"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C48" s="4">
         <v>3</v>
       </c>
-      <c r="D48" s="4">
-        <v>29</v>
-      </c>
+      <c r="D48" s="4"/>
       <c r="E48" s="18">
         <v>43061</v>
       </c>
@@ -1958,19 +1966,23 @@
         <v>12</v>
       </c>
       <c r="G48" s="4"/>
-      <c r="H48" s="5"/>
+      <c r="H48" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C49" s="4">
         <v>3</v>
       </c>
-      <c r="D49" s="4"/>
+      <c r="D49" s="4">
+        <v>29</v>
+      </c>
       <c r="E49" s="18">
         <v>43061</v>
       </c>
@@ -1978,199 +1990,253 @@
         <v>12</v>
       </c>
       <c r="G49" s="4"/>
-      <c r="H49" s="5" t="s">
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>31</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="4">
+        <v>3</v>
+      </c>
+      <c r="D50" s="4">
+        <v>29</v>
+      </c>
+      <c r="E50" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>32</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="4">
+        <v>3</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="13">
+    <row r="52" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="13">
         <v>33</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B52" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="15">
+      <c r="C52" s="15">
         <v>3</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="7"/>
-      <c r="H50" s="8" t="s">
+      <c r="E52" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="23" t="s">
+    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="25"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="10">
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="29"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="10">
         <v>34</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B55" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C55" s="11">
         <v>5</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="12"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
+      <c r="D55" s="11"/>
+      <c r="E55" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="12"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
         <v>35</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C56" s="4">
         <v>5</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="5" t="s">
+      <c r="D56" s="4"/>
+      <c r="E56" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="6">
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6">
         <v>36</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B57" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C57" s="7">
         <v>5</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="18">
-        <v>43061</v>
-      </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="8"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+      <c r="D57" s="7"/>
+      <c r="E57" s="18">
+        <v>43061</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="8"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="17">
         <v>37</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B59" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="23" t="s">
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="29"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="25"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="27" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="23" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="27" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="27" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A60:H60"/>
-    <mergeCell ref="A52:H52"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A39:H39"/>
     <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix puntos 38 39 40 41. falta probar 39 y 40
</commit_message>
<xml_diff>
--- a/DOCS/Pendientes Trader Prod.xlsx
+++ b/DOCS/Pendientes Trader Prod.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19095" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
   <si>
     <t>Pendientes Kraken Trader PROD</t>
   </si>
@@ -422,19 +422,22 @@
   </si>
   <si>
     <t>ver que es mas rentable/combeniente, subir a servidor en google cloud o ejecuta ren servido rpropio dedicado</t>
+  </si>
+  <si>
+    <t>PROBAR</t>
+  </si>
+  <si>
+    <t>Falta CREAR Campos en bbdd</t>
+  </si>
+  <si>
+    <t>evaluar si combiene comprar un fuente de internet alrtenatiba (BAN, SATELITAL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,7 +448,7 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="3" tint="0.399975585192419"/>
+      <color theme="3" tint="0.39994506668294322"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -458,159 +461,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,7 +471,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,192 +495,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -953,272 +625,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1265,58 +683,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1607,78 +997,79 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="64.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="12.7142857142857" customWidth="1"/>
-    <col min="8" max="8" width="94.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="94.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:8">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="18.75">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" ht="15.75"/>
-    <row r="3" ht="15.75" spans="1:8">
-      <c r="A3" s="3" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="15.75" spans="1:8">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:8" s="1" customFormat="1">
+      <c r="A4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1688,19 +1079,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="6">
         <v>43065</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="9">
+      <c r="A6" s="5">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1710,24 +1101,24 @@
         <v>1</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="6">
         <v>43063</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="1">
@@ -1736,19 +1127,19 @@
       <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="6">
         <v>43065</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="6">
         <v>43073</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="9">
+      <c r="A8" s="5">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1760,91 +1151,91 @@
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="6">
         <v>43089</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="10">
         <v>2</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="6">
         <v>43073</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="6">
         <v>43074</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="10">
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="10">
+      <c r="E10" s="6">
         <v>43074</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="12" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="10">
         <v>3</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="10">
+      <c r="E11" s="6">
         <v>43074</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="12" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="9">
+      <c r="A12" s="5">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1854,63 +1245,63 @@
         <v>2</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="6">
         <v>43066</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="10">
         <v>1</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="10">
+      <c r="E13" s="6">
         <v>43076</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="12"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="10">
         <v>2</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="10">
+      <c r="E14" s="6">
         <v>43078</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="12" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="15">
+      <c r="A15" s="11">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1922,19 +1313,19 @@
       <c r="D15" s="1">
         <v>4</v>
       </c>
-      <c r="E15" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F15" s="16" t="s">
+      <c r="E15" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="9">
+      <c r="A16" s="5">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1946,21 +1337,21 @@
       <c r="D16" s="1">
         <v>5</v>
       </c>
-      <c r="E16" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F16" s="11" t="s">
+      <c r="E16" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="6">
         <v>43095</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="9">
+      <c r="A17" s="5">
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1972,19 +1363,19 @@
       <c r="D17" s="1">
         <v>5</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="6">
         <v>43061</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="9">
+      <c r="A18" s="5">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1996,111 +1387,111 @@
       <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="6">
         <v>43061</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="10">
+      <c r="E19" s="6">
         <v>43078</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="6">
         <v>43091</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="10">
         <v>2</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="10">
         <v>8</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="6">
         <v>43074</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="10">
         <v>3</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="10">
+      <c r="D21" s="10"/>
+      <c r="E21" s="6">
         <v>43074</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="12" t="s">
         <v>35</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="10">
         <v>2</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="6">
         <v>43074</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="9">
+      <c r="A23" s="5">
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2112,21 +1503,21 @@
       <c r="D23" s="1">
         <v>8</v>
       </c>
-      <c r="E23" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F23" s="11" t="s">
+      <c r="E23" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="6">
         <v>43095</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="9">
+      <c r="A24" s="5">
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2138,19 +1529,19 @@
       <c r="D24" s="1">
         <v>8</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="6">
         <v>43061</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="9">
+      <c r="A25" s="5">
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2162,19 +1553,19 @@
       <c r="D25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="6">
         <v>43061</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="12" t="s">
+      <c r="H25" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="9">
+      <c r="A26" s="5">
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2186,19 +1577,19 @@
       <c r="D26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="6">
         <v>43061</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="12" t="s">
+      <c r="H26" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="9">
+      <c r="A27" s="5">
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2210,19 +1601,19 @@
       <c r="D27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="6">
         <v>43061</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="9">
+      <c r="A28" s="5">
         <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2232,21 +1623,21 @@
         <v>1</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F28" s="11" t="s">
+      <c r="E28" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="6">
         <v>43089</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="9">
+      <c r="A29" s="5">
         <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2258,21 +1649,21 @@
       <c r="D29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F29" s="11" t="s">
+      <c r="E29" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="6">
         <v>43089</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="9">
+      <c r="A30" s="5">
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2284,53 +1675,53 @@
       <c r="D30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F30" s="11" t="s">
+      <c r="E30" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="6">
         <v>43089</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="H30" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="9"/>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="5"/>
+      <c r="B31" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="10">
         <v>3</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="10">
+      <c r="E31" s="6">
         <v>43099</v>
       </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="12"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="9"/>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="5"/>
+      <c r="B32" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="10">
         <v>3</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="10">
+      <c r="E32" s="6">
         <v>43099</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="12"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="9">
+      <c r="A33" s="5">
         <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2340,19 +1731,19 @@
         <v>2</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="10">
+      <c r="E33" s="6">
         <v>43061</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="9">
+      <c r="A34" s="5">
         <v>18</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2362,19 +1753,19 @@
         <v>2</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="10">
+      <c r="E34" s="6">
         <v>43061</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="12" t="s">
+      <c r="H34" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="9">
+      <c r="A35" s="5">
         <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2384,19 +1775,19 @@
         <v>2</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="10">
+      <c r="E35" s="6">
         <v>43061</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="12" t="s">
+      <c r="H35" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="9">
+      <c r="A36" s="5">
         <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2408,56 +1799,55 @@
       <c r="D36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="6">
         <v>43061</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="12" t="s">
+      <c r="H36" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="37" ht="15.75" spans="1:8">
-      <c r="A37" s="17">
+    <row r="37" spans="1:8">
+      <c r="A37" s="13">
         <v>22</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="14">
         <v>2</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="18"/>
-      <c r="H37" s="19" t="s">
+      <c r="E37" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" ht="15.75"/>
-    <row r="39" ht="15.75" spans="1:8">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:8">
+      <c r="A39" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="8"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="9">
+      <c r="A40" s="5">
         <v>23</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2467,19 +1857,19 @@
         <v>4</v>
       </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="10">
+      <c r="E40" s="6">
         <v>43061</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G40" s="1"/>
-      <c r="H40" s="12" t="s">
+      <c r="H40" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="9">
+      <c r="A41" s="5">
         <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2489,19 +1879,19 @@
         <v>4</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="10">
+      <c r="E41" s="6">
         <v>43061</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="12" t="s">
+      <c r="H41" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="9">
+      <c r="A42" s="5">
         <v>25</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2511,19 +1901,19 @@
         <v>4</v>
       </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="10">
+      <c r="E42" s="6">
         <v>43061</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="12" t="s">
+      <c r="H42" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="9">
+      <c r="A43" s="5">
         <v>26</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2535,19 +1925,19 @@
       <c r="D43" s="1">
         <v>25</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="6">
         <v>43061</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="12" t="s">
+      <c r="H43" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="9">
+      <c r="A44" s="5">
         <v>27</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2559,56 +1949,55 @@
       <c r="D44" s="1">
         <v>25</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="6">
         <v>43061</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G44" s="1"/>
-      <c r="H44" s="12" t="s">
+      <c r="H44" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" ht="15.75" spans="1:8">
-      <c r="A45" s="17">
+    <row r="45" spans="1:8">
+      <c r="A45" s="13">
         <v>28</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="14">
         <v>4</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="14">
         <v>25</v>
       </c>
-      <c r="E45" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G45" s="18"/>
-      <c r="H45" s="19" t="s">
+      <c r="E45" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="14"/>
+      <c r="H45" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" ht="15.75"/>
-    <row r="47" ht="15.75" spans="1:8">
-      <c r="A47" s="6" t="s">
+    <row r="47" spans="1:8">
+      <c r="A47" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="8"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="34"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="9">
+      <c r="A48" s="5">
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2618,19 +2007,19 @@
         <v>3</v>
       </c>
       <c r="D48" s="1"/>
-      <c r="E48" s="10">
+      <c r="E48" s="6">
         <v>43061</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G48" s="1"/>
-      <c r="H48" s="12" t="s">
+      <c r="H48" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="9">
+      <c r="A49" s="5">
         <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2642,17 +2031,17 @@
       <c r="D49" s="1">
         <v>29</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="6">
         <v>43061</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="12"/>
+      <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="9">
+      <c r="A50" s="5">
         <v>31</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2664,17 +2053,17 @@
       <c r="D50" s="1">
         <v>29</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="6">
         <v>43061</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="12"/>
+      <c r="H50" s="8"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="9">
+      <c r="A51" s="5">
         <v>32</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2684,74 +2073,73 @@
         <v>3</v>
       </c>
       <c r="D51" s="1"/>
-      <c r="E51" s="10">
+      <c r="E51" s="6">
         <v>43061</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G51" s="1"/>
-      <c r="H51" s="12" t="s">
+      <c r="H51" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" ht="45.75" spans="1:8">
-      <c r="A52" s="20">
+    <row r="52" spans="1:8" ht="45">
+      <c r="A52" s="16">
         <v>33</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C52" s="22">
+      <c r="C52" s="18">
         <v>3</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D52" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E52" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F52" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G52" s="18"/>
-      <c r="H52" s="19" t="s">
+      <c r="E52" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G52" s="14"/>
+      <c r="H52" s="15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="53" ht="15.75"/>
-    <row r="54" ht="15.75" spans="1:8">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:8">
+      <c r="A54" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="8"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="34"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="24">
+      <c r="A55" s="20">
         <v>34</v>
       </c>
-      <c r="B55" s="25" t="s">
+      <c r="B55" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="25">
+      <c r="C55" s="21">
         <v>5</v>
       </c>
-      <c r="D55" s="25"/>
-      <c r="E55" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="26"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="22"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="9">
+      <c r="A56" s="5">
         <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2761,228 +2149,237 @@
         <v>5</v>
       </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="10">
+      <c r="E56" s="6">
         <v>43061</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="12" t="s">
+      <c r="H56" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="57" ht="15.75" spans="1:8">
-      <c r="A57" s="17">
+    <row r="57" spans="1:8">
+      <c r="A57" s="13">
         <v>36</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C57" s="14">
         <v>5</v>
       </c>
-      <c r="D57" s="18"/>
-      <c r="E57" s="10">
-        <v>43061</v>
-      </c>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="19"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="6">
+        <v>43061</v>
+      </c>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="15"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="27">
+      <c r="A59" s="23">
         <v>37</v>
       </c>
-      <c r="B59" s="27" t="s">
+      <c r="B59" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
-    </row>
-    <row r="61" ht="15.75"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+    </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="8"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="34"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="30"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G63" s="35">
+        <v>43210</v>
+      </c>
+      <c r="H63" s="26"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B64" s="29"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="29"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="30"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="35">
+        <v>43210</v>
+      </c>
+      <c r="F64" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="G64" s="25"/>
+      <c r="H64" s="37" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="29"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="30"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25"/>
+      <c r="H65" s="26"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B66" s="32"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="32"/>
-      <c r="H67" s="32"/>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="33" t="s">
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="35">
+        <v>43210</v>
+      </c>
+      <c r="F67" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="34" t="s">
+    <row r="71" spans="1:8">
+      <c r="A71" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="34" t="s">
+    <row r="72" spans="1:8">
+      <c r="A72" s="30" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="34" t="s">
+    <row r="73" spans="1:8">
+      <c r="A73" s="30" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="34" t="s">
+      <c r="A81" s="30" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
+    <row r="82" spans="1:1">
+      <c r="A82" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
         <v>134</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A62:H62"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A47:H47"/>
     <mergeCell ref="A54:H54"/>
-    <mergeCell ref="A62:H62"/>
   </mergeCells>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambios anteriores testeados y aprobados
</commit_message>
<xml_diff>
--- a/DOCS/Pendientes Trader Prod.xlsx
+++ b/DOCS/Pendientes Trader Prod.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="9000"/>
+    <workbookView windowWidth="19095" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137">
   <si>
     <t>Pendientes Kraken Trader PROD</t>
   </si>
@@ -376,6 +376,9 @@
     <t>guaedar maximo en bbdd, guardar "in-base" en bbdd</t>
   </si>
   <si>
+    <t>Marcha Blanca</t>
+  </si>
+  <si>
     <t>ajustar dinamicamante "deltaCHSaveProfit"= mma(10) del maximo*0,7</t>
   </si>
   <si>
@@ -421,23 +424,23 @@
     <t>comprar un monitor</t>
   </si>
   <si>
+    <t>evaluar si combiene comprar un fuente de internet alrtenatiba (BAN, SATELITAL)</t>
+  </si>
+  <si>
     <t>ver que es mas rentable/combeniente, subir a servidor en google cloud o ejecuta ren servido rpropio dedicado</t>
-  </si>
-  <si>
-    <t>PROBAR</t>
-  </si>
-  <si>
-    <t>Falta CREAR Campos en bbdd</t>
-  </si>
-  <si>
-    <t>evaluar si combiene comprar un fuente de internet alrtenatiba (BAN, SATELITAL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,7 +451,7 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="3" tint="0.39994506668294322"/>
+      <color theme="3" tint="0.399945066682943"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -461,8 +464,152 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,7 +618,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,18 +636,204 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -625,18 +958,272 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -669,44 +1256,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -997,79 +1610,80 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="64.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="94.5703125" customWidth="1"/>
+    <col min="2" max="2" width="64.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="10.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="12.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="10.5714285714286" customWidth="1"/>
+    <col min="8" max="8" width="94.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="31" t="s">
+    <row r="1" ht="18.75" spans="1:8">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" ht="15.75"/>
+    <row r="3" ht="15.75" spans="1:8">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1">
-      <c r="A4" s="32" t="s">
+    <row r="4" s="1" customFormat="1" ht="15.75" spans="1:8">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="5">
+      <c r="A5" s="9">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1079,19 +1693,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="10">
         <v>43065</v>
       </c>
-      <c r="H5" s="8"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="5">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1101,24 +1715,24 @@
         <v>1</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="10">
         <v>43063</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="1">
@@ -1127,19 +1741,19 @@
       <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="10">
         <v>43065</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="10">
         <v>43073</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1151,91 +1765,91 @@
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="10">
         <v>43089</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="14">
         <v>2</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="10">
         <v>43073</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="10">
         <v>43074</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="14">
         <v>3</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="6">
+      <c r="E10" s="10">
         <v>43074</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="8" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="14">
         <v>3</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="6">
+      <c r="E11" s="10">
         <v>43074</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="8" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="5">
+      <c r="A12" s="9">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1245,63 +1859,63 @@
         <v>2</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="10">
         <v>43066</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="14">
         <v>1</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="6">
+      <c r="E13" s="10">
         <v>43076</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="14">
         <v>2</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="6">
+      <c r="E14" s="10">
         <v>43078</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="8" t="s">
+      <c r="G14" s="10"/>
+      <c r="H14" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="11">
+      <c r="A15" s="15">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1313,19 +1927,19 @@
       <c r="D15" s="1">
         <v>4</v>
       </c>
-      <c r="E15" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="E15" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5">
+      <c r="A16" s="9">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1337,21 +1951,21 @@
       <c r="D16" s="1">
         <v>5</v>
       </c>
-      <c r="E16" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F16" s="7" t="s">
+      <c r="E16" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="10">
         <v>43095</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="5">
+      <c r="A17" s="9">
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1363,19 +1977,19 @@
       <c r="D17" s="1">
         <v>5</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="10">
         <v>43061</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="5">
+      <c r="A18" s="9">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1387,111 +2001,111 @@
       <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="10">
         <v>43061</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="6">
+      <c r="E19" s="10">
         <v>43078</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="10">
         <v>43091</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="14">
         <v>2</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="14">
         <v>8</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="10">
         <v>43074</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="14">
         <v>3</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="6">
+      <c r="D21" s="14"/>
+      <c r="E21" s="10">
         <v>43074</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="16" t="s">
         <v>35</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="14">
         <v>2</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="10">
         <v>43074</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="5">
+      <c r="A23" s="9">
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1503,21 +2117,21 @@
       <c r="D23" s="1">
         <v>8</v>
       </c>
-      <c r="E23" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F23" s="7" t="s">
+      <c r="E23" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="10">
         <v>43095</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="5">
+      <c r="A24" s="9">
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1529,19 +2143,19 @@
       <c r="D24" s="1">
         <v>8</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="10">
         <v>43061</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="5">
+      <c r="A25" s="9">
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1553,19 +2167,19 @@
       <c r="D25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="10">
         <v>43061</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="5">
+      <c r="A26" s="9">
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1577,19 +2191,19 @@
       <c r="D26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="10">
         <v>43061</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="5">
+      <c r="A27" s="9">
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1601,19 +2215,19 @@
       <c r="D27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="10">
         <v>43061</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="5">
+      <c r="A28" s="9">
         <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1623,21 +2237,21 @@
         <v>1</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F28" s="7" t="s">
+      <c r="E28" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="10">
         <v>43089</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="5">
+      <c r="A29" s="9">
         <v>15</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1649,21 +2263,21 @@
       <c r="D29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F29" s="7" t="s">
+      <c r="E29" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="10">
         <v>43089</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="5">
+      <c r="A30" s="9">
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1675,53 +2289,53 @@
       <c r="D30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F30" s="7" t="s">
+      <c r="E30" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="10">
         <v>43089</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="5"/>
-      <c r="B31" s="10" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="14">
         <v>3</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="6">
+      <c r="E31" s="10">
         <v>43099</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="8"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="5"/>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="14">
         <v>3</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="6">
+      <c r="E32" s="10">
         <v>43099</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="8"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="5">
+      <c r="A33" s="9">
         <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1731,19 +2345,19 @@
         <v>2</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="6">
+      <c r="E33" s="10">
         <v>43061</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="5">
+      <c r="A34" s="9">
         <v>18</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1753,19 +2367,19 @@
         <v>2</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="6">
+      <c r="E34" s="10">
         <v>43061</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="5">
+      <c r="A35" s="9">
         <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1775,19 +2389,19 @@
         <v>2</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="6">
+      <c r="E35" s="10">
         <v>43061</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="5">
+      <c r="A36" s="9">
         <v>21</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1799,55 +2413,56 @@
       <c r="D36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="10">
         <v>43061</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="13">
+    <row r="37" ht="15.75" spans="1:8">
+      <c r="A37" s="17">
         <v>22</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="18">
         <v>2</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F37" s="14" t="s">
+      <c r="E37" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F37" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="14"/>
-      <c r="H37" s="15" t="s">
+      <c r="G37" s="18"/>
+      <c r="H37" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="32" t="s">
+    <row r="38" ht="15.75"/>
+    <row r="39" ht="15.75" spans="1:8">
+      <c r="A39" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="34"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="5">
+      <c r="A40" s="9">
         <v>23</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1857,19 +2472,19 @@
         <v>4</v>
       </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="6">
+      <c r="E40" s="10">
         <v>43061</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G40" s="1"/>
-      <c r="H40" s="8" t="s">
+      <c r="H40" s="12" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="5">
+      <c r="A41" s="9">
         <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1879,19 +2494,19 @@
         <v>4</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="6">
+      <c r="E41" s="10">
         <v>43061</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="8" t="s">
+      <c r="H41" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="5">
+      <c r="A42" s="9">
         <v>25</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1901,19 +2516,19 @@
         <v>4</v>
       </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="6">
+      <c r="E42" s="10">
         <v>43061</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="5">
+      <c r="A43" s="9">
         <v>26</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1925,19 +2540,19 @@
       <c r="D43" s="1">
         <v>25</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="10">
         <v>43061</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="5">
+      <c r="A44" s="9">
         <v>27</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1949,55 +2564,56 @@
       <c r="D44" s="1">
         <v>25</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="10">
         <v>43061</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G44" s="1"/>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="13">
+    <row r="45" ht="15.75" spans="1:8">
+      <c r="A45" s="17">
         <v>28</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="18">
         <v>4</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="18">
         <v>25</v>
       </c>
-      <c r="E45" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F45" s="14" t="s">
+      <c r="E45" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="14"/>
-      <c r="H45" s="15" t="s">
+      <c r="G45" s="18"/>
+      <c r="H45" s="19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="32" t="s">
+    <row r="46" ht="15.75"/>
+    <row r="47" ht="15.75" spans="1:8">
+      <c r="A47" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="34"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="5">
+      <c r="A48" s="9">
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2007,19 +2623,19 @@
         <v>3</v>
       </c>
       <c r="D48" s="1"/>
-      <c r="E48" s="6">
+      <c r="E48" s="10">
         <v>43061</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G48" s="1"/>
-      <c r="H48" s="8" t="s">
+      <c r="H48" s="12" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="5">
+      <c r="A49" s="9">
         <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2031,17 +2647,17 @@
       <c r="D49" s="1">
         <v>29</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="10">
         <v>43061</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G49" s="1"/>
-      <c r="H49" s="8"/>
+      <c r="H49" s="12"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="5">
+      <c r="A50" s="9">
         <v>31</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2053,17 +2669,17 @@
       <c r="D50" s="1">
         <v>29</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="10">
         <v>43061</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="8"/>
+      <c r="H50" s="12"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="5">
+      <c r="A51" s="9">
         <v>32</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2073,73 +2689,74 @@
         <v>3</v>
       </c>
       <c r="D51" s="1"/>
-      <c r="E51" s="6">
+      <c r="E51" s="10">
         <v>43061</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G51" s="1"/>
-      <c r="H51" s="8" t="s">
+      <c r="H51" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="45">
-      <c r="A52" s="16">
+    <row r="52" ht="45.75" spans="1:8">
+      <c r="A52" s="20">
         <v>33</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C52" s="22">
         <v>3</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="E52" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F52" s="19" t="s">
+      <c r="E52" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F52" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="14"/>
-      <c r="H52" s="15" t="s">
+      <c r="G52" s="18"/>
+      <c r="H52" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="32" t="s">
+    <row r="53" ht="15.75"/>
+    <row r="54" ht="15.75" spans="1:8">
+      <c r="A54" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="34"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="20">
+      <c r="A55" s="24">
         <v>34</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="21">
+      <c r="C55" s="25">
         <v>5</v>
       </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="22"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="26"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="5">
+      <c r="A56" s="9">
         <v>35</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2149,108 +2766,109 @@
         <v>5</v>
       </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="6">
+      <c r="E56" s="10">
         <v>43061</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="8" t="s">
+      <c r="H56" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="13">
+    <row r="57" ht="15.75" spans="1:8">
+      <c r="A57" s="17">
         <v>36</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="18">
         <v>5</v>
       </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="6">
-        <v>43061</v>
-      </c>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="15"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="10">
+        <v>43061</v>
+      </c>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="19"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="23">
+      <c r="A59" s="27">
         <v>37</v>
       </c>
-      <c r="B59" s="23" t="s">
+      <c r="B59" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
-      <c r="F59" s="23"/>
-      <c r="G59" s="23"/>
-      <c r="H59" s="23"/>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="32" t="s">
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+    </row>
+    <row r="61" ht="15.75"/>
+    <row r="62" ht="15.75" spans="1:8">
+      <c r="A62" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B62" s="33"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="34"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="7" t="s">
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G63" s="35">
+      <c r="G63" s="29">
         <v>43210</v>
       </c>
-      <c r="H63" s="26"/>
+      <c r="H63" s="28"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="35">
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="29">
         <v>43210</v>
       </c>
-      <c r="F64" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="G64" s="25"/>
-      <c r="H64" s="37" t="s">
-        <v>136</v>
-      </c>
+      <c r="F64" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="G64" s="29">
+        <v>43210</v>
+      </c>
+      <c r="H64" s="31"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="26"/>
+      <c r="A65" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="27" t="s">
-        <v>120</v>
+      <c r="A66" s="32" t="s">
+        <v>121</v>
       </c>
       <c r="B66" s="28"/>
       <c r="C66" s="28"/>
@@ -2261,125 +2879,134 @@
       <c r="H66" s="28"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="27" t="s">
-        <v>121</v>
+      <c r="A67" s="32" t="s">
+        <v>122</v>
       </c>
       <c r="B67" s="28"/>
       <c r="C67" s="28"/>
       <c r="D67" s="28"/>
-      <c r="E67" s="35">
+      <c r="E67" s="29">
         <v>43210</v>
       </c>
-      <c r="F67" s="36" t="s">
-        <v>135</v>
+      <c r="F67" s="30" t="s">
+        <v>119</v>
       </c>
       <c r="G67" s="28"/>
       <c r="H67" s="28"/>
     </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+    <row r="68" spans="1:1">
+      <c r="A68" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="30" t="s">
+    <row r="71" spans="1:1">
+      <c r="A71" s="34" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="30" t="s">
+    <row r="72" spans="1:1">
+      <c r="A72" s="34" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="73" spans="1:1">
+      <c r="A73" s="34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="30" t="s">
-        <v>133</v>
+      <c r="A81" s="34" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="30" t="s">
-        <v>137</v>
+      <c r="A82" s="34" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A62:H62"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A47:H47"/>
     <mergeCell ref="A54:H54"/>
+    <mergeCell ref="A62:H62"/>
   </mergeCells>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>